<commit_message>
Se agregan validacion a la carga de programacion de obra
</commit_message>
<xml_diff>
--- a/asivamosffie.web/asivamosffie/src/assets/files/Programacion_De_Obra.xlsx
+++ b/asivamosffie.web/asivamosffie/src/assets/files/Programacion_De_Obra.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Proyectos\Desktop\Proyectos\FFIE\Casos de Uso\Plantillas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Diego\Trabajo\Ivolucion\Fuentes\Version\así vamos FFIE\asivamosffie.web\asivamosffie\src\assets\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E38F6A0-C22D-4187-B3FF-13369C945A43}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EB1F509-52D8-4F08-8227-20F87CC9B346}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A293A7F9-D452-4580-B76E-8023013B04D6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{A293A7F9-D452-4580-B76E-8023013B04D6}"/>
   </bookViews>
   <sheets>
     <sheet name="Programación de obra" sheetId="1" r:id="rId1"/>
@@ -99,16 +99,7 @@
     <t>Capítulo 2</t>
   </si>
   <si>
-    <t>i (Item)</t>
-  </si>
-  <si>
-    <t>SC (Subcapítulo)</t>
-  </si>
-  <si>
     <t>Capítulo 1</t>
-  </si>
-  <si>
-    <t>C (Capítulo)</t>
   </si>
   <si>
     <t>Duración total de actividad (Días)</t>
@@ -127,6 +118,15 @@
   </si>
   <si>
     <t>Marca de ruta crítica (Solo debe marcarse con 1)</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>SC</t>
+  </si>
+  <si>
+    <t>I</t>
   </si>
 </sst>
 </file>
@@ -843,40 +843,40 @@
   <dimension ref="A1:FW201"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.5" style="1" customWidth="1"/>
-    <col min="2" max="2" width="54.09765625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="54.125" style="1" customWidth="1"/>
     <col min="3" max="3" width="13.5" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12.19921875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.25" style="1" customWidth="1"/>
     <col min="6" max="6" width="11" style="1" customWidth="1"/>
-    <col min="7" max="162" width="3.69921875" style="1" customWidth="1"/>
-    <col min="163" max="174" width="3.8984375" style="1" customWidth="1"/>
+    <col min="7" max="162" width="3.75" style="1" customWidth="1"/>
+    <col min="163" max="174" width="3.875" style="1" customWidth="1"/>
     <col min="175" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:179" s="23" customFormat="1" ht="49.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:179" s="23" customFormat="1" ht="49.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="D1" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="D1" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="E1" s="26" t="s">
-        <v>32</v>
-      </c>
       <c r="F1" s="25" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G1" s="25">
         <v>1</v>
@@ -1388,12 +1388,12 @@
       <c r="FV1" s="24"/>
       <c r="FW1" s="24"/>
     </row>
-    <row r="2" spans="1:179" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:179" x14ac:dyDescent="0.2">
       <c r="A2" s="22" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C2" s="15"/>
       <c r="D2" s="14"/>
@@ -1571,9 +1571,9 @@
       <c r="FQ2" s="20"/>
       <c r="FR2" s="19"/>
     </row>
-    <row r="3" spans="1:179" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:179" x14ac:dyDescent="0.2">
       <c r="A3" s="16" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="B3" s="17" t="s">
         <v>4</v>
@@ -1754,9 +1754,9 @@
       <c r="FQ3" s="11"/>
       <c r="FR3" s="10"/>
     </row>
-    <row r="4" spans="1:179" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:179" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>1</v>
@@ -1937,9 +1937,9 @@
       <c r="FQ4" s="11"/>
       <c r="FR4" s="10"/>
     </row>
-    <row r="5" spans="1:179" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:179" x14ac:dyDescent="0.2">
       <c r="A5" s="16" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>0</v>
@@ -2120,7 +2120,7 @@
       <c r="FQ5" s="11"/>
       <c r="FR5" s="10"/>
     </row>
-    <row r="6" spans="1:179" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:179" x14ac:dyDescent="0.2">
       <c r="A6" s="16"/>
       <c r="B6" s="17" t="s">
         <v>3</v>
@@ -2301,7 +2301,7 @@
       <c r="FQ6" s="11"/>
       <c r="FR6" s="10"/>
     </row>
-    <row r="7" spans="1:179" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:179" x14ac:dyDescent="0.2">
       <c r="A7" s="16"/>
       <c r="B7" s="8" t="s">
         <v>1</v>
@@ -2482,7 +2482,7 @@
       <c r="FQ7" s="11"/>
       <c r="FR7" s="10"/>
     </row>
-    <row r="8" spans="1:179" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:179" x14ac:dyDescent="0.2">
       <c r="A8" s="16"/>
       <c r="B8" s="8" t="s">
         <v>0</v>
@@ -2663,7 +2663,7 @@
       <c r="FQ8" s="11"/>
       <c r="FR8" s="10"/>
     </row>
-    <row r="9" spans="1:179" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:179" x14ac:dyDescent="0.2">
       <c r="A9" s="16"/>
       <c r="B9" s="17" t="s">
         <v>2</v>
@@ -2844,7 +2844,7 @@
       <c r="FQ9" s="11"/>
       <c r="FR9" s="10"/>
     </row>
-    <row r="10" spans="1:179" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:179" x14ac:dyDescent="0.2">
       <c r="A10" s="16"/>
       <c r="B10" s="8" t="s">
         <v>1</v>
@@ -3025,7 +3025,7 @@
       <c r="FQ10" s="11"/>
       <c r="FR10" s="10"/>
     </row>
-    <row r="11" spans="1:179" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:179" x14ac:dyDescent="0.2">
       <c r="A11" s="16"/>
       <c r="B11" s="8" t="s">
         <v>0</v>
@@ -3206,7 +3206,7 @@
       <c r="FQ11" s="11"/>
       <c r="FR11" s="10"/>
     </row>
-    <row r="12" spans="1:179" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:179" x14ac:dyDescent="0.2">
       <c r="A12" s="16"/>
       <c r="B12" s="18" t="s">
         <v>23</v>
@@ -3387,7 +3387,7 @@
       <c r="FQ12" s="11"/>
       <c r="FR12" s="10"/>
     </row>
-    <row r="13" spans="1:179" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:179" x14ac:dyDescent="0.2">
       <c r="A13" s="16"/>
       <c r="B13" s="17" t="s">
         <v>4</v>
@@ -3568,7 +3568,7 @@
       <c r="FQ13" s="11"/>
       <c r="FR13" s="10"/>
     </row>
-    <row r="14" spans="1:179" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:179" x14ac:dyDescent="0.2">
       <c r="A14" s="16"/>
       <c r="B14" s="8" t="s">
         <v>1</v>
@@ -3749,7 +3749,7 @@
       <c r="FQ14" s="11"/>
       <c r="FR14" s="10"/>
     </row>
-    <row r="15" spans="1:179" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:179" x14ac:dyDescent="0.2">
       <c r="A15" s="16"/>
       <c r="B15" s="8" t="s">
         <v>0</v>
@@ -3930,7 +3930,7 @@
       <c r="FQ15" s="11"/>
       <c r="FR15" s="10"/>
     </row>
-    <row r="16" spans="1:179" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:179" x14ac:dyDescent="0.2">
       <c r="A16" s="16"/>
       <c r="B16" s="17" t="s">
         <v>3</v>
@@ -4111,7 +4111,7 @@
       <c r="FQ16" s="11"/>
       <c r="FR16" s="10"/>
     </row>
-    <row r="17" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A17" s="16"/>
       <c r="B17" s="8" t="s">
         <v>1</v>
@@ -4292,7 +4292,7 @@
       <c r="FQ17" s="11"/>
       <c r="FR17" s="10"/>
     </row>
-    <row r="18" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A18" s="16"/>
       <c r="B18" s="8" t="s">
         <v>0</v>
@@ -4473,7 +4473,7 @@
       <c r="FQ18" s="11"/>
       <c r="FR18" s="10"/>
     </row>
-    <row r="19" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A19" s="16"/>
       <c r="B19" s="17" t="s">
         <v>2</v>
@@ -4654,7 +4654,7 @@
       <c r="FQ19" s="11"/>
       <c r="FR19" s="10"/>
     </row>
-    <row r="20" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A20" s="16"/>
       <c r="B20" s="8" t="s">
         <v>1</v>
@@ -4835,7 +4835,7 @@
       <c r="FQ20" s="11"/>
       <c r="FR20" s="10"/>
     </row>
-    <row r="21" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A21" s="16"/>
       <c r="B21" s="8" t="s">
         <v>0</v>
@@ -5016,7 +5016,7 @@
       <c r="FQ21" s="11"/>
       <c r="FR21" s="10"/>
     </row>
-    <row r="22" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A22" s="16"/>
       <c r="B22" s="18" t="s">
         <v>22</v>
@@ -5197,7 +5197,7 @@
       <c r="FQ22" s="11"/>
       <c r="FR22" s="10"/>
     </row>
-    <row r="23" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A23" s="16"/>
       <c r="B23" s="17" t="s">
         <v>4</v>
@@ -5378,7 +5378,7 @@
       <c r="FQ23" s="11"/>
       <c r="FR23" s="10"/>
     </row>
-    <row r="24" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A24" s="16"/>
       <c r="B24" s="8" t="s">
         <v>1</v>
@@ -5559,7 +5559,7 @@
       <c r="FQ24" s="11"/>
       <c r="FR24" s="10"/>
     </row>
-    <row r="25" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A25" s="16"/>
       <c r="B25" s="8" t="s">
         <v>0</v>
@@ -5740,7 +5740,7 @@
       <c r="FQ25" s="11"/>
       <c r="FR25" s="10"/>
     </row>
-    <row r="26" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A26" s="16"/>
       <c r="B26" s="17" t="s">
         <v>3</v>
@@ -5921,7 +5921,7 @@
       <c r="FQ26" s="11"/>
       <c r="FR26" s="10"/>
     </row>
-    <row r="27" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A27" s="16"/>
       <c r="B27" s="8" t="s">
         <v>1</v>
@@ -6102,7 +6102,7 @@
       <c r="FQ27" s="11"/>
       <c r="FR27" s="10"/>
     </row>
-    <row r="28" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A28" s="16"/>
       <c r="B28" s="8" t="s">
         <v>0</v>
@@ -6283,7 +6283,7 @@
       <c r="FQ28" s="11"/>
       <c r="FR28" s="10"/>
     </row>
-    <row r="29" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A29" s="16"/>
       <c r="B29" s="17" t="s">
         <v>2</v>
@@ -6464,7 +6464,7 @@
       <c r="FQ29" s="11"/>
       <c r="FR29" s="10"/>
     </row>
-    <row r="30" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A30" s="16"/>
       <c r="B30" s="8" t="s">
         <v>1</v>
@@ -6645,7 +6645,7 @@
       <c r="FQ30" s="11"/>
       <c r="FR30" s="10"/>
     </row>
-    <row r="31" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A31" s="16"/>
       <c r="B31" s="8" t="s">
         <v>0</v>
@@ -6826,7 +6826,7 @@
       <c r="FQ31" s="11"/>
       <c r="FR31" s="10"/>
     </row>
-    <row r="32" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A32" s="16"/>
       <c r="B32" s="18" t="s">
         <v>21</v>
@@ -7007,7 +7007,7 @@
       <c r="FQ32" s="11"/>
       <c r="FR32" s="10"/>
     </row>
-    <row r="33" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A33" s="16"/>
       <c r="B33" s="17" t="s">
         <v>4</v>
@@ -7188,7 +7188,7 @@
       <c r="FQ33" s="11"/>
       <c r="FR33" s="10"/>
     </row>
-    <row r="34" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A34" s="16"/>
       <c r="B34" s="8" t="s">
         <v>1</v>
@@ -7369,7 +7369,7 @@
       <c r="FQ34" s="11"/>
       <c r="FR34" s="10"/>
     </row>
-    <row r="35" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A35" s="16"/>
       <c r="B35" s="8" t="s">
         <v>0</v>
@@ -7550,7 +7550,7 @@
       <c r="FQ35" s="11"/>
       <c r="FR35" s="10"/>
     </row>
-    <row r="36" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A36" s="16"/>
       <c r="B36" s="17" t="s">
         <v>3</v>
@@ -7731,7 +7731,7 @@
       <c r="FQ36" s="11"/>
       <c r="FR36" s="10"/>
     </row>
-    <row r="37" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A37" s="16"/>
       <c r="B37" s="8" t="s">
         <v>1</v>
@@ -7912,7 +7912,7 @@
       <c r="FQ37" s="11"/>
       <c r="FR37" s="10"/>
     </row>
-    <row r="38" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A38" s="16"/>
       <c r="B38" s="8" t="s">
         <v>0</v>
@@ -8093,7 +8093,7 @@
       <c r="FQ38" s="11"/>
       <c r="FR38" s="10"/>
     </row>
-    <row r="39" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A39" s="16"/>
       <c r="B39" s="17" t="s">
         <v>2</v>
@@ -8274,7 +8274,7 @@
       <c r="FQ39" s="11"/>
       <c r="FR39" s="10"/>
     </row>
-    <row r="40" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A40" s="16"/>
       <c r="B40" s="8" t="s">
         <v>1</v>
@@ -8455,7 +8455,7 @@
       <c r="FQ40" s="11"/>
       <c r="FR40" s="10"/>
     </row>
-    <row r="41" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A41" s="16"/>
       <c r="B41" s="8" t="s">
         <v>0</v>
@@ -8636,7 +8636,7 @@
       <c r="FQ41" s="11"/>
       <c r="FR41" s="10"/>
     </row>
-    <row r="42" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A42" s="16"/>
       <c r="B42" s="18" t="s">
         <v>20</v>
@@ -8817,7 +8817,7 @@
       <c r="FQ42" s="11"/>
       <c r="FR42" s="10"/>
     </row>
-    <row r="43" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A43" s="16"/>
       <c r="B43" s="17" t="s">
         <v>4</v>
@@ -8998,7 +8998,7 @@
       <c r="FQ43" s="11"/>
       <c r="FR43" s="10"/>
     </row>
-    <row r="44" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A44" s="16"/>
       <c r="B44" s="8" t="s">
         <v>1</v>
@@ -9179,7 +9179,7 @@
       <c r="FQ44" s="11"/>
       <c r="FR44" s="10"/>
     </row>
-    <row r="45" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A45" s="16"/>
       <c r="B45" s="8" t="s">
         <v>0</v>
@@ -9360,7 +9360,7 @@
       <c r="FQ45" s="11"/>
       <c r="FR45" s="10"/>
     </row>
-    <row r="46" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A46" s="16"/>
       <c r="B46" s="17" t="s">
         <v>3</v>
@@ -9541,7 +9541,7 @@
       <c r="FQ46" s="11"/>
       <c r="FR46" s="10"/>
     </row>
-    <row r="47" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A47" s="16"/>
       <c r="B47" s="8" t="s">
         <v>1</v>
@@ -9722,7 +9722,7 @@
       <c r="FQ47" s="11"/>
       <c r="FR47" s="10"/>
     </row>
-    <row r="48" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A48" s="16"/>
       <c r="B48" s="8" t="s">
         <v>0</v>
@@ -9903,7 +9903,7 @@
       <c r="FQ48" s="11"/>
       <c r="FR48" s="10"/>
     </row>
-    <row r="49" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A49" s="16"/>
       <c r="B49" s="17" t="s">
         <v>2</v>
@@ -10084,7 +10084,7 @@
       <c r="FQ49" s="11"/>
       <c r="FR49" s="10"/>
     </row>
-    <row r="50" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A50" s="16"/>
       <c r="B50" s="8" t="s">
         <v>1</v>
@@ -10265,7 +10265,7 @@
       <c r="FQ50" s="11"/>
       <c r="FR50" s="10"/>
     </row>
-    <row r="51" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A51" s="16"/>
       <c r="B51" s="8" t="s">
         <v>0</v>
@@ -10446,7 +10446,7 @@
       <c r="FQ51" s="11"/>
       <c r="FR51" s="10"/>
     </row>
-    <row r="52" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A52" s="16"/>
       <c r="B52" s="18" t="s">
         <v>19</v>
@@ -10627,7 +10627,7 @@
       <c r="FQ52" s="11"/>
       <c r="FR52" s="10"/>
     </row>
-    <row r="53" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A53" s="16"/>
       <c r="B53" s="17" t="s">
         <v>4</v>
@@ -10808,7 +10808,7 @@
       <c r="FQ53" s="11"/>
       <c r="FR53" s="10"/>
     </row>
-    <row r="54" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A54" s="16"/>
       <c r="B54" s="8" t="s">
         <v>1</v>
@@ -10989,7 +10989,7 @@
       <c r="FQ54" s="11"/>
       <c r="FR54" s="10"/>
     </row>
-    <row r="55" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A55" s="16"/>
       <c r="B55" s="8" t="s">
         <v>0</v>
@@ -11170,7 +11170,7 @@
       <c r="FQ55" s="11"/>
       <c r="FR55" s="10"/>
     </row>
-    <row r="56" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A56" s="16"/>
       <c r="B56" s="17" t="s">
         <v>3</v>
@@ -11351,7 +11351,7 @@
       <c r="FQ56" s="11"/>
       <c r="FR56" s="10"/>
     </row>
-    <row r="57" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A57" s="16"/>
       <c r="B57" s="8" t="s">
         <v>1</v>
@@ -11532,7 +11532,7 @@
       <c r="FQ57" s="11"/>
       <c r="FR57" s="10"/>
     </row>
-    <row r="58" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A58" s="16"/>
       <c r="B58" s="8" t="s">
         <v>0</v>
@@ -11713,7 +11713,7 @@
       <c r="FQ58" s="11"/>
       <c r="FR58" s="10"/>
     </row>
-    <row r="59" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A59" s="16"/>
       <c r="B59" s="17" t="s">
         <v>2</v>
@@ -11894,7 +11894,7 @@
       <c r="FQ59" s="11"/>
       <c r="FR59" s="10"/>
     </row>
-    <row r="60" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A60" s="16"/>
       <c r="B60" s="8" t="s">
         <v>1</v>
@@ -12075,7 +12075,7 @@
       <c r="FQ60" s="11"/>
       <c r="FR60" s="10"/>
     </row>
-    <row r="61" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A61" s="16"/>
       <c r="B61" s="8" t="s">
         <v>0</v>
@@ -12256,7 +12256,7 @@
       <c r="FQ61" s="11"/>
       <c r="FR61" s="10"/>
     </row>
-    <row r="62" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A62" s="16"/>
       <c r="B62" s="18" t="s">
         <v>18</v>
@@ -12437,7 +12437,7 @@
       <c r="FQ62" s="11"/>
       <c r="FR62" s="10"/>
     </row>
-    <row r="63" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A63" s="16"/>
       <c r="B63" s="17" t="s">
         <v>4</v>
@@ -12618,7 +12618,7 @@
       <c r="FQ63" s="11"/>
       <c r="FR63" s="10"/>
     </row>
-    <row r="64" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A64" s="16"/>
       <c r="B64" s="8" t="s">
         <v>1</v>
@@ -12799,7 +12799,7 @@
       <c r="FQ64" s="11"/>
       <c r="FR64" s="10"/>
     </row>
-    <row r="65" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A65" s="16"/>
       <c r="B65" s="8" t="s">
         <v>0</v>
@@ -12980,7 +12980,7 @@
       <c r="FQ65" s="11"/>
       <c r="FR65" s="10"/>
     </row>
-    <row r="66" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A66" s="16"/>
       <c r="B66" s="17" t="s">
         <v>3</v>
@@ -13161,7 +13161,7 @@
       <c r="FQ66" s="11"/>
       <c r="FR66" s="10"/>
     </row>
-    <row r="67" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A67" s="16"/>
       <c r="B67" s="8" t="s">
         <v>1</v>
@@ -13342,7 +13342,7 @@
       <c r="FQ67" s="11"/>
       <c r="FR67" s="10"/>
     </row>
-    <row r="68" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A68" s="16"/>
       <c r="B68" s="8" t="s">
         <v>0</v>
@@ -13523,7 +13523,7 @@
       <c r="FQ68" s="11"/>
       <c r="FR68" s="10"/>
     </row>
-    <row r="69" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A69" s="16"/>
       <c r="B69" s="17" t="s">
         <v>2</v>
@@ -13704,7 +13704,7 @@
       <c r="FQ69" s="11"/>
       <c r="FR69" s="10"/>
     </row>
-    <row r="70" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A70" s="16"/>
       <c r="B70" s="8" t="s">
         <v>1</v>
@@ -13885,7 +13885,7 @@
       <c r="FQ70" s="11"/>
       <c r="FR70" s="10"/>
     </row>
-    <row r="71" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A71" s="16"/>
       <c r="B71" s="8" t="s">
         <v>0</v>
@@ -14066,7 +14066,7 @@
       <c r="FQ71" s="11"/>
       <c r="FR71" s="10"/>
     </row>
-    <row r="72" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A72" s="16"/>
       <c r="B72" s="18" t="s">
         <v>17</v>
@@ -14247,7 +14247,7 @@
       <c r="FQ72" s="11"/>
       <c r="FR72" s="10"/>
     </row>
-    <row r="73" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A73" s="16"/>
       <c r="B73" s="17" t="s">
         <v>4</v>
@@ -14428,7 +14428,7 @@
       <c r="FQ73" s="11"/>
       <c r="FR73" s="10"/>
     </row>
-    <row r="74" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A74" s="16"/>
       <c r="B74" s="8" t="s">
         <v>1</v>
@@ -14609,7 +14609,7 @@
       <c r="FQ74" s="11"/>
       <c r="FR74" s="10"/>
     </row>
-    <row r="75" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A75" s="16"/>
       <c r="B75" s="8" t="s">
         <v>0</v>
@@ -14790,7 +14790,7 @@
       <c r="FQ75" s="11"/>
       <c r="FR75" s="10"/>
     </row>
-    <row r="76" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A76" s="16"/>
       <c r="B76" s="17" t="s">
         <v>3</v>
@@ -14971,7 +14971,7 @@
       <c r="FQ76" s="11"/>
       <c r="FR76" s="10"/>
     </row>
-    <row r="77" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A77" s="16"/>
       <c r="B77" s="8" t="s">
         <v>1</v>
@@ -15152,7 +15152,7 @@
       <c r="FQ77" s="11"/>
       <c r="FR77" s="10"/>
     </row>
-    <row r="78" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A78" s="16"/>
       <c r="B78" s="8" t="s">
         <v>0</v>
@@ -15333,7 +15333,7 @@
       <c r="FQ78" s="11"/>
       <c r="FR78" s="10"/>
     </row>
-    <row r="79" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A79" s="16"/>
       <c r="B79" s="17" t="s">
         <v>2</v>
@@ -15514,7 +15514,7 @@
       <c r="FQ79" s="11"/>
       <c r="FR79" s="10"/>
     </row>
-    <row r="80" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A80" s="16"/>
       <c r="B80" s="8" t="s">
         <v>1</v>
@@ -15695,7 +15695,7 @@
       <c r="FQ80" s="11"/>
       <c r="FR80" s="10"/>
     </row>
-    <row r="81" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A81" s="16"/>
       <c r="B81" s="8" t="s">
         <v>0</v>
@@ -15876,7 +15876,7 @@
       <c r="FQ81" s="11"/>
       <c r="FR81" s="10"/>
     </row>
-    <row r="82" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A82" s="16"/>
       <c r="B82" s="18" t="s">
         <v>16</v>
@@ -16057,7 +16057,7 @@
       <c r="FQ82" s="11"/>
       <c r="FR82" s="10"/>
     </row>
-    <row r="83" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A83" s="16"/>
       <c r="B83" s="17" t="s">
         <v>4</v>
@@ -16238,7 +16238,7 @@
       <c r="FQ83" s="11"/>
       <c r="FR83" s="10"/>
     </row>
-    <row r="84" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A84" s="16"/>
       <c r="B84" s="8" t="s">
         <v>1</v>
@@ -16419,7 +16419,7 @@
       <c r="FQ84" s="11"/>
       <c r="FR84" s="10"/>
     </row>
-    <row r="85" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A85" s="16"/>
       <c r="B85" s="8" t="s">
         <v>0</v>
@@ -16600,7 +16600,7 @@
       <c r="FQ85" s="11"/>
       <c r="FR85" s="10"/>
     </row>
-    <row r="86" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A86" s="16"/>
       <c r="B86" s="17" t="s">
         <v>3</v>
@@ -16781,7 +16781,7 @@
       <c r="FQ86" s="11"/>
       <c r="FR86" s="10"/>
     </row>
-    <row r="87" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A87" s="16"/>
       <c r="B87" s="8" t="s">
         <v>1</v>
@@ -16962,7 +16962,7 @@
       <c r="FQ87" s="11"/>
       <c r="FR87" s="10"/>
     </row>
-    <row r="88" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A88" s="16"/>
       <c r="B88" s="8" t="s">
         <v>0</v>
@@ -17143,7 +17143,7 @@
       <c r="FQ88" s="11"/>
       <c r="FR88" s="10"/>
     </row>
-    <row r="89" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A89" s="16"/>
       <c r="B89" s="17" t="s">
         <v>2</v>
@@ -17324,7 +17324,7 @@
       <c r="FQ89" s="11"/>
       <c r="FR89" s="10"/>
     </row>
-    <row r="90" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A90" s="16"/>
       <c r="B90" s="8" t="s">
         <v>1</v>
@@ -17505,7 +17505,7 @@
       <c r="FQ90" s="11"/>
       <c r="FR90" s="10"/>
     </row>
-    <row r="91" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A91" s="16"/>
       <c r="B91" s="8" t="s">
         <v>0</v>
@@ -17686,7 +17686,7 @@
       <c r="FQ91" s="11"/>
       <c r="FR91" s="10"/>
     </row>
-    <row r="92" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A92" s="16"/>
       <c r="B92" s="18" t="s">
         <v>15</v>
@@ -17867,7 +17867,7 @@
       <c r="FQ92" s="11"/>
       <c r="FR92" s="10"/>
     </row>
-    <row r="93" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A93" s="16"/>
       <c r="B93" s="17" t="s">
         <v>4</v>
@@ -18048,7 +18048,7 @@
       <c r="FQ93" s="11"/>
       <c r="FR93" s="10"/>
     </row>
-    <row r="94" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A94" s="16"/>
       <c r="B94" s="8" t="s">
         <v>1</v>
@@ -18229,7 +18229,7 @@
       <c r="FQ94" s="11"/>
       <c r="FR94" s="10"/>
     </row>
-    <row r="95" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A95" s="16"/>
       <c r="B95" s="8" t="s">
         <v>0</v>
@@ -18410,7 +18410,7 @@
       <c r="FQ95" s="11"/>
       <c r="FR95" s="10"/>
     </row>
-    <row r="96" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A96" s="16"/>
       <c r="B96" s="17" t="s">
         <v>3</v>
@@ -18591,7 +18591,7 @@
       <c r="FQ96" s="11"/>
       <c r="FR96" s="10"/>
     </row>
-    <row r="97" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A97" s="16"/>
       <c r="B97" s="8" t="s">
         <v>1</v>
@@ -18772,7 +18772,7 @@
       <c r="FQ97" s="11"/>
       <c r="FR97" s="10"/>
     </row>
-    <row r="98" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A98" s="16"/>
       <c r="B98" s="8" t="s">
         <v>0</v>
@@ -18953,7 +18953,7 @@
       <c r="FQ98" s="11"/>
       <c r="FR98" s="10"/>
     </row>
-    <row r="99" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A99" s="16"/>
       <c r="B99" s="17" t="s">
         <v>2</v>
@@ -19134,7 +19134,7 @@
       <c r="FQ99" s="11"/>
       <c r="FR99" s="10"/>
     </row>
-    <row r="100" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A100" s="16"/>
       <c r="B100" s="8" t="s">
         <v>1</v>
@@ -19315,7 +19315,7 @@
       <c r="FQ100" s="11"/>
       <c r="FR100" s="10"/>
     </row>
-    <row r="101" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A101" s="16"/>
       <c r="B101" s="8" t="s">
         <v>0</v>
@@ -19496,7 +19496,7 @@
       <c r="FQ101" s="11"/>
       <c r="FR101" s="10"/>
     </row>
-    <row r="102" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A102" s="16"/>
       <c r="B102" s="18" t="s">
         <v>14</v>
@@ -19677,7 +19677,7 @@
       <c r="FQ102" s="11"/>
       <c r="FR102" s="10"/>
     </row>
-    <row r="103" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A103" s="16"/>
       <c r="B103" s="17" t="s">
         <v>4</v>
@@ -19858,7 +19858,7 @@
       <c r="FQ103" s="11"/>
       <c r="FR103" s="10"/>
     </row>
-    <row r="104" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A104" s="16"/>
       <c r="B104" s="8" t="s">
         <v>1</v>
@@ -20039,7 +20039,7 @@
       <c r="FQ104" s="11"/>
       <c r="FR104" s="10"/>
     </row>
-    <row r="105" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A105" s="16"/>
       <c r="B105" s="8" t="s">
         <v>0</v>
@@ -20220,7 +20220,7 @@
       <c r="FQ105" s="11"/>
       <c r="FR105" s="10"/>
     </row>
-    <row r="106" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A106" s="16"/>
       <c r="B106" s="17" t="s">
         <v>3</v>
@@ -20401,7 +20401,7 @@
       <c r="FQ106" s="11"/>
       <c r="FR106" s="10"/>
     </row>
-    <row r="107" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A107" s="16"/>
       <c r="B107" s="8" t="s">
         <v>1</v>
@@ -20582,7 +20582,7 @@
       <c r="FQ107" s="11"/>
       <c r="FR107" s="10"/>
     </row>
-    <row r="108" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A108" s="16"/>
       <c r="B108" s="8" t="s">
         <v>0</v>
@@ -20763,7 +20763,7 @@
       <c r="FQ108" s="11"/>
       <c r="FR108" s="10"/>
     </row>
-    <row r="109" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A109" s="16"/>
       <c r="B109" s="17" t="s">
         <v>2</v>
@@ -20944,7 +20944,7 @@
       <c r="FQ109" s="11"/>
       <c r="FR109" s="10"/>
     </row>
-    <row r="110" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A110" s="16"/>
       <c r="B110" s="8" t="s">
         <v>1</v>
@@ -21125,7 +21125,7 @@
       <c r="FQ110" s="11"/>
       <c r="FR110" s="10"/>
     </row>
-    <row r="111" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A111" s="16"/>
       <c r="B111" s="8" t="s">
         <v>0</v>
@@ -21306,7 +21306,7 @@
       <c r="FQ111" s="11"/>
       <c r="FR111" s="10"/>
     </row>
-    <row r="112" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A112" s="16"/>
       <c r="B112" s="18" t="s">
         <v>13</v>
@@ -21487,7 +21487,7 @@
       <c r="FQ112" s="11"/>
       <c r="FR112" s="10"/>
     </row>
-    <row r="113" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A113" s="16"/>
       <c r="B113" s="17" t="s">
         <v>4</v>
@@ -21668,7 +21668,7 @@
       <c r="FQ113" s="11"/>
       <c r="FR113" s="10"/>
     </row>
-    <row r="114" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A114" s="16"/>
       <c r="B114" s="8" t="s">
         <v>1</v>
@@ -21849,7 +21849,7 @@
       <c r="FQ114" s="11"/>
       <c r="FR114" s="10"/>
     </row>
-    <row r="115" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A115" s="16"/>
       <c r="B115" s="8" t="s">
         <v>0</v>
@@ -22030,7 +22030,7 @@
       <c r="FQ115" s="11"/>
       <c r="FR115" s="10"/>
     </row>
-    <row r="116" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A116" s="16"/>
       <c r="B116" s="17" t="s">
         <v>3</v>
@@ -22211,7 +22211,7 @@
       <c r="FQ116" s="11"/>
       <c r="FR116" s="10"/>
     </row>
-    <row r="117" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A117" s="16"/>
       <c r="B117" s="8" t="s">
         <v>1</v>
@@ -22392,7 +22392,7 @@
       <c r="FQ117" s="11"/>
       <c r="FR117" s="10"/>
     </row>
-    <row r="118" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A118" s="16"/>
       <c r="B118" s="8" t="s">
         <v>0</v>
@@ -22573,7 +22573,7 @@
       <c r="FQ118" s="11"/>
       <c r="FR118" s="10"/>
     </row>
-    <row r="119" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A119" s="16"/>
       <c r="B119" s="17" t="s">
         <v>2</v>
@@ -22754,7 +22754,7 @@
       <c r="FQ119" s="11"/>
       <c r="FR119" s="10"/>
     </row>
-    <row r="120" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A120" s="16"/>
       <c r="B120" s="8" t="s">
         <v>1</v>
@@ -22935,7 +22935,7 @@
       <c r="FQ120" s="11"/>
       <c r="FR120" s="10"/>
     </row>
-    <row r="121" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A121" s="16"/>
       <c r="B121" s="8" t="s">
         <v>0</v>
@@ -23116,7 +23116,7 @@
       <c r="FQ121" s="11"/>
       <c r="FR121" s="10"/>
     </row>
-    <row r="122" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A122" s="16"/>
       <c r="B122" s="18" t="s">
         <v>12</v>
@@ -23297,7 +23297,7 @@
       <c r="FQ122" s="11"/>
       <c r="FR122" s="10"/>
     </row>
-    <row r="123" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A123" s="16"/>
       <c r="B123" s="17" t="s">
         <v>4</v>
@@ -23478,7 +23478,7 @@
       <c r="FQ123" s="11"/>
       <c r="FR123" s="10"/>
     </row>
-    <row r="124" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A124" s="16"/>
       <c r="B124" s="8" t="s">
         <v>1</v>
@@ -23659,7 +23659,7 @@
       <c r="FQ124" s="11"/>
       <c r="FR124" s="10"/>
     </row>
-    <row r="125" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A125" s="16"/>
       <c r="B125" s="8" t="s">
         <v>0</v>
@@ -23840,7 +23840,7 @@
       <c r="FQ125" s="11"/>
       <c r="FR125" s="10"/>
     </row>
-    <row r="126" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A126" s="16"/>
       <c r="B126" s="17" t="s">
         <v>3</v>
@@ -24021,7 +24021,7 @@
       <c r="FQ126" s="11"/>
       <c r="FR126" s="10"/>
     </row>
-    <row r="127" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A127" s="16"/>
       <c r="B127" s="8" t="s">
         <v>1</v>
@@ -24202,7 +24202,7 @@
       <c r="FQ127" s="11"/>
       <c r="FR127" s="10"/>
     </row>
-    <row r="128" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A128" s="16"/>
       <c r="B128" s="8" t="s">
         <v>0</v>
@@ -24383,7 +24383,7 @@
       <c r="FQ128" s="11"/>
       <c r="FR128" s="10"/>
     </row>
-    <row r="129" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A129" s="16"/>
       <c r="B129" s="17" t="s">
         <v>2</v>
@@ -24564,7 +24564,7 @@
       <c r="FQ129" s="11"/>
       <c r="FR129" s="10"/>
     </row>
-    <row r="130" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A130" s="16"/>
       <c r="B130" s="8" t="s">
         <v>1</v>
@@ -24745,7 +24745,7 @@
       <c r="FQ130" s="11"/>
       <c r="FR130" s="10"/>
     </row>
-    <row r="131" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A131" s="16"/>
       <c r="B131" s="8" t="s">
         <v>0</v>
@@ -24926,7 +24926,7 @@
       <c r="FQ131" s="11"/>
       <c r="FR131" s="10"/>
     </row>
-    <row r="132" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A132" s="16"/>
       <c r="B132" s="18" t="s">
         <v>11</v>
@@ -25107,7 +25107,7 @@
       <c r="FQ132" s="11"/>
       <c r="FR132" s="10"/>
     </row>
-    <row r="133" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A133" s="16"/>
       <c r="B133" s="17" t="s">
         <v>4</v>
@@ -25288,7 +25288,7 @@
       <c r="FQ133" s="11"/>
       <c r="FR133" s="10"/>
     </row>
-    <row r="134" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A134" s="16"/>
       <c r="B134" s="8" t="s">
         <v>1</v>
@@ -25469,7 +25469,7 @@
       <c r="FQ134" s="11"/>
       <c r="FR134" s="10"/>
     </row>
-    <row r="135" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A135" s="16"/>
       <c r="B135" s="8" t="s">
         <v>0</v>
@@ -25650,7 +25650,7 @@
       <c r="FQ135" s="11"/>
       <c r="FR135" s="10"/>
     </row>
-    <row r="136" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A136" s="16"/>
       <c r="B136" s="17" t="s">
         <v>3</v>
@@ -25831,7 +25831,7 @@
       <c r="FQ136" s="11"/>
       <c r="FR136" s="10"/>
     </row>
-    <row r="137" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A137" s="16"/>
       <c r="B137" s="8" t="s">
         <v>1</v>
@@ -26012,7 +26012,7 @@
       <c r="FQ137" s="11"/>
       <c r="FR137" s="10"/>
     </row>
-    <row r="138" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A138" s="16"/>
       <c r="B138" s="8" t="s">
         <v>0</v>
@@ -26193,7 +26193,7 @@
       <c r="FQ138" s="11"/>
       <c r="FR138" s="10"/>
     </row>
-    <row r="139" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A139" s="16"/>
       <c r="B139" s="17" t="s">
         <v>2</v>
@@ -26374,7 +26374,7 @@
       <c r="FQ139" s="11"/>
       <c r="FR139" s="10"/>
     </row>
-    <row r="140" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A140" s="16"/>
       <c r="B140" s="8" t="s">
         <v>1</v>
@@ -26555,7 +26555,7 @@
       <c r="FQ140" s="11"/>
       <c r="FR140" s="10"/>
     </row>
-    <row r="141" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A141" s="16"/>
       <c r="B141" s="8" t="s">
         <v>0</v>
@@ -26736,7 +26736,7 @@
       <c r="FQ141" s="11"/>
       <c r="FR141" s="10"/>
     </row>
-    <row r="142" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A142" s="16"/>
       <c r="B142" s="18" t="s">
         <v>10</v>
@@ -26917,7 +26917,7 @@
       <c r="FQ142" s="11"/>
       <c r="FR142" s="10"/>
     </row>
-    <row r="143" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A143" s="16"/>
       <c r="B143" s="17" t="s">
         <v>4</v>
@@ -27098,7 +27098,7 @@
       <c r="FQ143" s="11"/>
       <c r="FR143" s="10"/>
     </row>
-    <row r="144" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A144" s="16"/>
       <c r="B144" s="8" t="s">
         <v>1</v>
@@ -27279,7 +27279,7 @@
       <c r="FQ144" s="11"/>
       <c r="FR144" s="10"/>
     </row>
-    <row r="145" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A145" s="16"/>
       <c r="B145" s="8" t="s">
         <v>0</v>
@@ -27460,7 +27460,7 @@
       <c r="FQ145" s="11"/>
       <c r="FR145" s="10"/>
     </row>
-    <row r="146" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A146" s="16"/>
       <c r="B146" s="17" t="s">
         <v>3</v>
@@ -27641,7 +27641,7 @@
       <c r="FQ146" s="11"/>
       <c r="FR146" s="10"/>
     </row>
-    <row r="147" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A147" s="16"/>
       <c r="B147" s="8" t="s">
         <v>1</v>
@@ -27822,7 +27822,7 @@
       <c r="FQ147" s="11"/>
       <c r="FR147" s="10"/>
     </row>
-    <row r="148" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A148" s="16"/>
       <c r="B148" s="8" t="s">
         <v>0</v>
@@ -28003,7 +28003,7 @@
       <c r="FQ148" s="11"/>
       <c r="FR148" s="10"/>
     </row>
-    <row r="149" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A149" s="16"/>
       <c r="B149" s="17" t="s">
         <v>2</v>
@@ -28184,7 +28184,7 @@
       <c r="FQ149" s="11"/>
       <c r="FR149" s="10"/>
     </row>
-    <row r="150" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A150" s="16"/>
       <c r="B150" s="8" t="s">
         <v>1</v>
@@ -28365,7 +28365,7 @@
       <c r="FQ150" s="11"/>
       <c r="FR150" s="10"/>
     </row>
-    <row r="151" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A151" s="16"/>
       <c r="B151" s="8" t="s">
         <v>0</v>
@@ -28546,7 +28546,7 @@
       <c r="FQ151" s="11"/>
       <c r="FR151" s="10"/>
     </row>
-    <row r="152" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A152" s="16"/>
       <c r="B152" s="18" t="s">
         <v>9</v>
@@ -28727,7 +28727,7 @@
       <c r="FQ152" s="11"/>
       <c r="FR152" s="10"/>
     </row>
-    <row r="153" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A153" s="16"/>
       <c r="B153" s="17" t="s">
         <v>4</v>
@@ -28908,7 +28908,7 @@
       <c r="FQ153" s="11"/>
       <c r="FR153" s="10"/>
     </row>
-    <row r="154" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A154" s="16"/>
       <c r="B154" s="8" t="s">
         <v>1</v>
@@ -29089,7 +29089,7 @@
       <c r="FQ154" s="11"/>
       <c r="FR154" s="10"/>
     </row>
-    <row r="155" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A155" s="16"/>
       <c r="B155" s="8" t="s">
         <v>0</v>
@@ -29270,7 +29270,7 @@
       <c r="FQ155" s="11"/>
       <c r="FR155" s="10"/>
     </row>
-    <row r="156" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A156" s="16"/>
       <c r="B156" s="17" t="s">
         <v>3</v>
@@ -29451,7 +29451,7 @@
       <c r="FQ156" s="11"/>
       <c r="FR156" s="10"/>
     </row>
-    <row r="157" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A157" s="16"/>
       <c r="B157" s="8" t="s">
         <v>1</v>
@@ -29632,7 +29632,7 @@
       <c r="FQ157" s="11"/>
       <c r="FR157" s="10"/>
     </row>
-    <row r="158" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A158" s="16"/>
       <c r="B158" s="8" t="s">
         <v>0</v>
@@ -29813,7 +29813,7 @@
       <c r="FQ158" s="11"/>
       <c r="FR158" s="10"/>
     </row>
-    <row r="159" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A159" s="16"/>
       <c r="B159" s="17" t="s">
         <v>2</v>
@@ -29994,7 +29994,7 @@
       <c r="FQ159" s="11"/>
       <c r="FR159" s="10"/>
     </row>
-    <row r="160" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A160" s="16"/>
       <c r="B160" s="8" t="s">
         <v>1</v>
@@ -30175,7 +30175,7 @@
       <c r="FQ160" s="11"/>
       <c r="FR160" s="10"/>
     </row>
-    <row r="161" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A161" s="16"/>
       <c r="B161" s="8" t="s">
         <v>0</v>
@@ -30356,7 +30356,7 @@
       <c r="FQ161" s="11"/>
       <c r="FR161" s="10"/>
     </row>
-    <row r="162" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A162" s="16"/>
       <c r="B162" s="18" t="s">
         <v>8</v>
@@ -30537,7 +30537,7 @@
       <c r="FQ162" s="11"/>
       <c r="FR162" s="10"/>
     </row>
-    <row r="163" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A163" s="16"/>
       <c r="B163" s="17" t="s">
         <v>4</v>
@@ -30718,7 +30718,7 @@
       <c r="FQ163" s="11"/>
       <c r="FR163" s="10"/>
     </row>
-    <row r="164" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A164" s="16"/>
       <c r="B164" s="8" t="s">
         <v>1</v>
@@ -30899,7 +30899,7 @@
       <c r="FQ164" s="11"/>
       <c r="FR164" s="10"/>
     </row>
-    <row r="165" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A165" s="16"/>
       <c r="B165" s="8" t="s">
         <v>0</v>
@@ -31080,7 +31080,7 @@
       <c r="FQ165" s="11"/>
       <c r="FR165" s="10"/>
     </row>
-    <row r="166" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A166" s="16"/>
       <c r="B166" s="17" t="s">
         <v>3</v>
@@ -31261,7 +31261,7 @@
       <c r="FQ166" s="11"/>
       <c r="FR166" s="10"/>
     </row>
-    <row r="167" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A167" s="16"/>
       <c r="B167" s="8" t="s">
         <v>1</v>
@@ -31442,7 +31442,7 @@
       <c r="FQ167" s="11"/>
       <c r="FR167" s="10"/>
     </row>
-    <row r="168" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A168" s="16"/>
       <c r="B168" s="8" t="s">
         <v>0</v>
@@ -31623,7 +31623,7 @@
       <c r="FQ168" s="11"/>
       <c r="FR168" s="10"/>
     </row>
-    <row r="169" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A169" s="16"/>
       <c r="B169" s="17" t="s">
         <v>2</v>
@@ -31804,7 +31804,7 @@
       <c r="FQ169" s="11"/>
       <c r="FR169" s="10"/>
     </row>
-    <row r="170" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A170" s="16"/>
       <c r="B170" s="8" t="s">
         <v>1</v>
@@ -31985,7 +31985,7 @@
       <c r="FQ170" s="11"/>
       <c r="FR170" s="10"/>
     </row>
-    <row r="171" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A171" s="16"/>
       <c r="B171" s="8" t="s">
         <v>0</v>
@@ -32166,7 +32166,7 @@
       <c r="FQ171" s="11"/>
       <c r="FR171" s="10"/>
     </row>
-    <row r="172" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A172" s="16"/>
       <c r="B172" s="18" t="s">
         <v>7</v>
@@ -32347,7 +32347,7 @@
       <c r="FQ172" s="11"/>
       <c r="FR172" s="10"/>
     </row>
-    <row r="173" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A173" s="16"/>
       <c r="B173" s="17" t="s">
         <v>4</v>
@@ -32528,7 +32528,7 @@
       <c r="FQ173" s="11"/>
       <c r="FR173" s="10"/>
     </row>
-    <row r="174" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A174" s="16"/>
       <c r="B174" s="8" t="s">
         <v>1</v>
@@ -32709,7 +32709,7 @@
       <c r="FQ174" s="11"/>
       <c r="FR174" s="10"/>
     </row>
-    <row r="175" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A175" s="16"/>
       <c r="B175" s="8" t="s">
         <v>0</v>
@@ -32890,7 +32890,7 @@
       <c r="FQ175" s="11"/>
       <c r="FR175" s="10"/>
     </row>
-    <row r="176" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A176" s="16"/>
       <c r="B176" s="17" t="s">
         <v>3</v>
@@ -33071,7 +33071,7 @@
       <c r="FQ176" s="11"/>
       <c r="FR176" s="10"/>
     </row>
-    <row r="177" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A177" s="16"/>
       <c r="B177" s="8" t="s">
         <v>1</v>
@@ -33252,7 +33252,7 @@
       <c r="FQ177" s="11"/>
       <c r="FR177" s="10"/>
     </row>
-    <row r="178" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A178" s="16"/>
       <c r="B178" s="8" t="s">
         <v>0</v>
@@ -33433,7 +33433,7 @@
       <c r="FQ178" s="11"/>
       <c r="FR178" s="10"/>
     </row>
-    <row r="179" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A179" s="16"/>
       <c r="B179" s="17" t="s">
         <v>2</v>
@@ -33614,7 +33614,7 @@
       <c r="FQ179" s="11"/>
       <c r="FR179" s="10"/>
     </row>
-    <row r="180" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A180" s="16"/>
       <c r="B180" s="8" t="s">
         <v>1</v>
@@ -33795,7 +33795,7 @@
       <c r="FQ180" s="11"/>
       <c r="FR180" s="10"/>
     </row>
-    <row r="181" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A181" s="16"/>
       <c r="B181" s="8" t="s">
         <v>0</v>
@@ -33976,7 +33976,7 @@
       <c r="FQ181" s="11"/>
       <c r="FR181" s="10"/>
     </row>
-    <row r="182" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A182" s="16"/>
       <c r="B182" s="18" t="s">
         <v>6</v>
@@ -34157,7 +34157,7 @@
       <c r="FQ182" s="11"/>
       <c r="FR182" s="10"/>
     </row>
-    <row r="183" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A183" s="16"/>
       <c r="B183" s="17" t="s">
         <v>4</v>
@@ -34338,7 +34338,7 @@
       <c r="FQ183" s="11"/>
       <c r="FR183" s="10"/>
     </row>
-    <row r="184" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A184" s="16"/>
       <c r="B184" s="8" t="s">
         <v>1</v>
@@ -34519,7 +34519,7 @@
       <c r="FQ184" s="11"/>
       <c r="FR184" s="10"/>
     </row>
-    <row r="185" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A185" s="16"/>
       <c r="B185" s="8" t="s">
         <v>0</v>
@@ -34700,7 +34700,7 @@
       <c r="FQ185" s="11"/>
       <c r="FR185" s="10"/>
     </row>
-    <row r="186" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A186" s="16"/>
       <c r="B186" s="17" t="s">
         <v>3</v>
@@ -34881,7 +34881,7 @@
       <c r="FQ186" s="11"/>
       <c r="FR186" s="10"/>
     </row>
-    <row r="187" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A187" s="16"/>
       <c r="B187" s="8" t="s">
         <v>1</v>
@@ -35062,7 +35062,7 @@
       <c r="FQ187" s="11"/>
       <c r="FR187" s="10"/>
     </row>
-    <row r="188" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A188" s="16"/>
       <c r="B188" s="8" t="s">
         <v>0</v>
@@ -35243,7 +35243,7 @@
       <c r="FQ188" s="11"/>
       <c r="FR188" s="10"/>
     </row>
-    <row r="189" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A189" s="16"/>
       <c r="B189" s="17" t="s">
         <v>2</v>
@@ -35424,7 +35424,7 @@
       <c r="FQ189" s="11"/>
       <c r="FR189" s="10"/>
     </row>
-    <row r="190" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A190" s="16"/>
       <c r="B190" s="8" t="s">
         <v>1</v>
@@ -35605,7 +35605,7 @@
       <c r="FQ190" s="11"/>
       <c r="FR190" s="10"/>
     </row>
-    <row r="191" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A191" s="16"/>
       <c r="B191" s="8" t="s">
         <v>0</v>
@@ -35786,7 +35786,7 @@
       <c r="FQ191" s="11"/>
       <c r="FR191" s="10"/>
     </row>
-    <row r="192" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A192" s="16"/>
       <c r="B192" s="18" t="s">
         <v>5</v>
@@ -35967,7 +35967,7 @@
       <c r="FQ192" s="11"/>
       <c r="FR192" s="10"/>
     </row>
-    <row r="193" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A193" s="16"/>
       <c r="B193" s="17" t="s">
         <v>4</v>
@@ -36148,7 +36148,7 @@
       <c r="FQ193" s="11"/>
       <c r="FR193" s="10"/>
     </row>
-    <row r="194" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A194" s="16"/>
       <c r="B194" s="8" t="s">
         <v>1</v>
@@ -36157,7 +36157,7 @@
       <c r="D194" s="14"/>
       <c r="E194" s="14"/>
       <c r="F194" s="13">
-        <f t="shared" ref="F194:F225" si="6">SUM(G194:FR194)</f>
+        <f t="shared" ref="F194:F201" si="6">SUM(G194:FR194)</f>
         <v>0</v>
       </c>
       <c r="G194" s="12"/>
@@ -36329,7 +36329,7 @@
       <c r="FQ194" s="11"/>
       <c r="FR194" s="10"/>
     </row>
-    <row r="195" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A195" s="16"/>
       <c r="B195" s="8" t="s">
         <v>0</v>
@@ -36510,7 +36510,7 @@
       <c r="FQ195" s="11"/>
       <c r="FR195" s="10"/>
     </row>
-    <row r="196" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A196" s="16"/>
       <c r="B196" s="17" t="s">
         <v>3</v>
@@ -36691,7 +36691,7 @@
       <c r="FQ196" s="11"/>
       <c r="FR196" s="10"/>
     </row>
-    <row r="197" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A197" s="16"/>
       <c r="B197" s="8" t="s">
         <v>1</v>
@@ -36872,7 +36872,7 @@
       <c r="FQ197" s="11"/>
       <c r="FR197" s="10"/>
     </row>
-    <row r="198" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A198" s="16"/>
       <c r="B198" s="8" t="s">
         <v>0</v>
@@ -37053,7 +37053,7 @@
       <c r="FQ198" s="11"/>
       <c r="FR198" s="10"/>
     </row>
-    <row r="199" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A199" s="16"/>
       <c r="B199" s="17" t="s">
         <v>2</v>
@@ -37234,7 +37234,7 @@
       <c r="FQ199" s="11"/>
       <c r="FR199" s="10"/>
     </row>
-    <row r="200" spans="1:174" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:174" x14ac:dyDescent="0.2">
       <c r="A200" s="16"/>
       <c r="B200" s="8" t="s">
         <v>1</v>
@@ -37415,7 +37415,7 @@
       <c r="FQ200" s="11"/>
       <c r="FR200" s="10"/>
     </row>
-    <row r="201" spans="1:174" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:174" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A201" s="9"/>
       <c r="B201" s="8" t="s">
         <v>0</v>
@@ -37602,8 +37602,8 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C201" xr:uid="{6D8D0A19-4139-4D1A-8BCB-E04BE78FC4AC}">
       <formula1>"1"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A201" xr:uid="{09F46021-1201-40CB-82D7-F8DE47C7EDCD}">
-      <formula1>"C (Capítulo),SC (Subcapítulo),i (Item)"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1048576" xr:uid="{90F5CA6D-52BA-481A-BA41-7B41ED883CD0}">
+      <formula1>"C,SC,I"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>